<commit_message>
Added Analyse concurrentielle to RapportDeTravail
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50567644-783C-4E87-96B5-ABFD5A4E2E28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -113,12 +112,24 @@
   </si>
   <si>
     <t>Mise à jour de la planification initiale pour prendre en compte les exigeances du cahier des charges</t>
+  </si>
+  <si>
+    <t>Analyse concurentielle, j'installe plusieurs application de tracking fitness sur mon téléphone et je note les fonctionnalités que je trouve intéressantes ainsi que celles que je trouve moins inéressantes</t>
+  </si>
+  <si>
+    <t>Continuation de l'analyse concurentielle, à partir des tests que j'ai faits sur les différents applications, je remplis un tableau comparatif des fonctionnalités intégrées par les applications</t>
+  </si>
+  <si>
+    <t>Définition de l'audience de l'application. Il s'agit ici de définir les personnes qui pouraient être amenés à utilisé l'application qui sera développer</t>
+  </si>
+  <si>
+    <t>0..5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
@@ -440,24 +451,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -474,7 +485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -489,7 +500,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -504,7 +515,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -519,7 +530,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -534,7 +545,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -549,7 +560,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -566,7 +577,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -581,7 +592,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -598,7 +609,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -615,7 +626,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -630,7 +641,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -647,7 +658,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -662,7 +673,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -677,7 +688,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -692,7 +703,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -707,7 +718,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -722,614 +733,644 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
-      <c r="D18" s="2"/>
+    <row r="18" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>1.5</v>
+      </c>
+      <c r="D18" s="2">
+        <v>43509</v>
+      </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
-      <c r="D19" s="2"/>
+    <row r="19" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="2">
+        <v>43509</v>
+      </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
-      <c r="D20" s="2"/>
+    <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="2">
+        <v>43509</v>
+      </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="D21" s="2"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="D23" s="2"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="D24" s="2"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="D25" s="2"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="D26" s="2"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="D28" s="2"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="D31" s="2"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="D32" s="2"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="D33" s="2"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="D34" s="2"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="D35" s="2"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="D36" s="2"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="D37" s="2"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="D38" s="2"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="D39" s="2"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="D40" s="2"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="D41" s="2"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="D42" s="2"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="D43" s="2"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="D44" s="2"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="D45" s="2"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="D46" s="2"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="D47" s="2"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="D48" s="2"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="D49" s="2"/>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="D50" s="2"/>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="D51" s="2"/>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="D52" s="2"/>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="D53" s="2"/>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="D54" s="2"/>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="D55" s="2"/>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="D56" s="2"/>
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="D57" s="2"/>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="D58" s="2"/>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="D59" s="2"/>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="D60" s="2"/>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="D61" s="2"/>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="D62" s="2"/>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="D63" s="2"/>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="D64" s="2"/>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="D65" s="2"/>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="D66" s="2"/>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
       <c r="D67" s="2"/>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="D68" s="2"/>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="D69" s="2"/>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="D70" s="2"/>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="D71" s="2"/>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="D72" s="2"/>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="D73" s="2"/>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="D74" s="2"/>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
       <c r="D75" s="2"/>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="D76" s="2"/>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="D77" s="2"/>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="D78" s="2"/>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
       <c r="D79" s="2"/>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="D80" s="2"/>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="D81" s="2"/>
       <c r="E81" s="1"/>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="D82" s="2"/>
       <c r="E82" s="1"/>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="D83" s="2"/>
       <c r="E83" s="1"/>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="D84" s="2"/>
       <c r="E84" s="1"/>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="D85" s="2"/>
       <c r="E85" s="1"/>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
       <c r="D86" s="2"/>
       <c r="E86" s="1"/>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="D87" s="2"/>
       <c r="E87" s="1"/>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
       <c r="D88" s="2"/>
       <c r="E88" s="1"/>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
       <c r="D89" s="2"/>
       <c r="E89" s="1"/>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="1"/>
       <c r="D90" s="2"/>
       <c r="E90" s="1"/>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
       <c r="D91" s="2"/>
       <c r="E91" s="1"/>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
       <c r="D92" s="2"/>
       <c r="E92" s="1"/>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="1"/>
       <c r="D93" s="2"/>
       <c r="E93" s="1"/>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
       <c r="D94" s="2"/>
       <c r="E94" s="1"/>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="1"/>
       <c r="D95" s="2"/>
       <c r="E95" s="1"/>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
       <c r="D96" s="2"/>
       <c r="E96" s="1"/>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
       <c r="D97" s="2"/>
       <c r="E97" s="1"/>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="D98" s="2"/>
       <c r="E98" s="1"/>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
       <c r="D99" s="2"/>
       <c r="E99" s="1"/>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
       <c r="D100" s="2"/>
       <c r="E100" s="1"/>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B101" s="1"/>
       <c r="D101" s="2"/>
       <c r="E101" s="1"/>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B102" s="1"/>
       <c r="D102" s="2"/>
       <c r="E102" s="1"/>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B103" s="1"/>
       <c r="D103" s="2"/>
       <c r="E103" s="1"/>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B104" s="1"/>
       <c r="D104" s="2"/>
       <c r="E104" s="1"/>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="D105" s="2"/>
       <c r="E105" s="1"/>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="D106" s="2"/>
       <c r="E106" s="1"/>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="D107" s="2"/>
       <c r="E107" s="1"/>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="D108" s="2"/>
       <c r="E108" s="1"/>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B109" s="1"/>
       <c r="D109" s="2"/>
       <c r="E109" s="1"/>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
       <c r="D110" s="2"/>
       <c r="E110" s="1"/>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B111" s="1"/>
       <c r="D111" s="2"/>
       <c r="E111" s="1"/>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B112" s="1"/>
       <c r="D112" s="2"/>
       <c r="E112" s="1"/>
     </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B113" s="1"/>
       <c r="D113" s="2"/>
       <c r="E113" s="1"/>
     </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B114" s="1"/>
       <c r="D114" s="2"/>
       <c r="E114" s="1"/>
     </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B115" s="1"/>
       <c r="D115" s="2"/>
       <c r="E115" s="1"/>
     </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B116" s="1"/>
       <c r="D116" s="2"/>
       <c r="E116" s="1"/>
     </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B117" s="1"/>
       <c r="D117" s="2"/>
       <c r="E117" s="1"/>
     </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B118" s="1"/>
       <c r="D118" s="2"/>
       <c r="E118" s="1"/>
     </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B119" s="1"/>
       <c r="D119" s="2"/>
       <c r="E119" s="1"/>
     </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B120" s="1"/>
       <c r="D120" s="2"/>
       <c r="E120" s="1"/>
     </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B121" s="1"/>
       <c r="D121" s="2"/>
       <c r="E121" s="1"/>
     </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B122" s="1"/>
       <c r="D122" s="2"/>
       <c r="E122" s="1"/>
     </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B123" s="1"/>
       <c r="D123" s="2"/>
       <c r="E123" s="1"/>
     </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B124" s="1"/>
       <c r="D124" s="2"/>
       <c r="E124" s="1"/>
     </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B125" s="1"/>
       <c r="D125" s="2"/>
       <c r="E125" s="1"/>
     </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B126" s="1"/>
       <c r="D126" s="2"/>
       <c r="E126" s="1"/>
     </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B127" s="1"/>
       <c r="D127" s="2"/>
     </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B128" s="1"/>
       <c r="D128" s="2"/>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" s="1"/>
       <c r="D129" s="2"/>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="1"/>
       <c r="D130" s="2"/>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" s="1"/>
       <c r="D131" s="2"/>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" s="1"/>
       <c r="D132" s="2"/>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" s="1"/>
       <c r="D133" s="2"/>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" s="1"/>
       <c r="D134" s="2"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" s="1"/>
       <c r="D135" s="2"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B136" s="1"/>
       <c r="D136" s="2"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" s="1"/>
       <c r="D137" s="2"/>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" s="1"/>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" s="1"/>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B140" s="1"/>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B141" s="1"/>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B142" s="1"/>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B143" s="1"/>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B144" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added PHILIBERT_PlanificationDetaillee, Updated Analyse concurrentielle, Added définition de l'audience, Added Analyse de faisabilité
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Refléxion sur la mise en service d'une authentification stateless</t>
   </si>
   <si>
-    <t>C'est la première fois que je rencontre le problème de réalisé une authentification stateless, qui ne repose donc sur aucun stockage côté serveur. Je trouve que certains problèmes sont plus simplement résolus lorsque une tel architecture est mise en place, comme par exemple, l'attribution de scope aux ressources. D'autres problèmes sont cependant présent avec une authetification stateless</t>
-  </si>
-  <si>
     <t>Conception</t>
   </si>
   <si>
@@ -123,7 +120,19 @@
     <t>Définition de l'audience de l'application. Il s'agit ici de définir les personnes qui pouraient être amenés à utilisé l'application qui sera développer</t>
   </si>
   <si>
-    <t>0..5</t>
+    <t xml:space="preserve">Écriture de l'analyse de faisabilité, je défini la faisabilité système ainsi que la faisabilité logicielle, aucun problème de faisabilité ne devrait être rencontré </t>
+  </si>
+  <si>
+    <t>Je termine mon analyse concurrentielle, je termine de remplir mon tableau comparatif et j'ajoute encore quelques points à comparés</t>
+  </si>
+  <si>
+    <t>Début de la plannification détaillée</t>
+  </si>
+  <si>
+    <t>C'est la première fois que je rencontre le problème de réalisé une authentification stateless, qui ne repose donc sur aucun stockage côté serveur. Je trouve que certains problèmes sont plus simplement résolus lorsque une tel architecture est mise en place, comme par exemple, l'attribution de scope aux ressources. D'autres problèmes sont cependant présent avec une authetification stateless, comme la mise en place de JSON Web Tokens</t>
+  </si>
+  <si>
+    <t>Je commence la plannification détaillée avec comme modèle la plannification initiale, il y a certains point que je n'arrive pas à détailler plus, vu que ces points sont nouveau pour moi, je n'arrive donc pas à déterminer toutes les étapes nécessaire pour effectuer ces tâches dans la plannifaction à ce moment du projet</t>
   </si>
 </sst>
 </file>
@@ -455,8 +464,8 @@
   <dimension ref="A1:E144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +601,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -606,7 +615,7 @@
         <v>43503</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -614,7 +623,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>0.5</v>
@@ -623,15 +632,15 @@
         <v>43504</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="C11">
         <v>0.5</v>
@@ -646,7 +655,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>0.5</v>
@@ -655,15 +664,15 @@
         <v>43504</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -675,10 +684,10 @@
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -693,7 +702,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15">
         <v>0.5</v>
@@ -708,7 +717,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16">
         <v>0.5</v>
@@ -723,7 +732,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17">
         <v>0.5</v>
@@ -733,12 +742,12 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>1.5</v>
@@ -753,7 +762,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19">
         <v>0.5</v>
@@ -763,35 +772,67 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="C20">
+        <v>0.5</v>
       </c>
       <c r="D20" s="2">
         <v>43509</v>
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="D21" s="2"/>
+    <row r="21" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="2">
+        <v>43509</v>
+      </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="D22" s="2"/>
+    <row r="22" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="2">
+        <v>43509</v>
+      </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
+    <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23">
+        <v>1.5</v>
+      </c>
+      <c r="D23" s="2">
+        <v>43509</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>

</xml_diff>

<commit_message>
Added MLD, Added Flow Diagram for Account Creation
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -133,6 +133,24 @@
   </si>
   <si>
     <t>Je commence la plannification détaillée avec comme modèle la plannification initiale, il y a certains point que je n'arrive pas à détailler plus, vu que ces points sont nouveau pour moi, je n'arrive donc pas à déterminer toutes les étapes nécessaire pour effectuer ces tâches dans la plannifaction à ce moment du projet</t>
+  </si>
+  <si>
+    <t>Réalisation</t>
+  </si>
+  <si>
+    <t>Réinitialisation de la carte SD du raspberry Pi avec une nouvelle installation de Raspbian</t>
+  </si>
+  <si>
+    <t>Mise à jour du MLD avec les informations récoltées depuis le cahier des charges, modification du MCD pour prendre en compte la table d'abonnement que peux obtenir un utilisateur</t>
+  </si>
+  <si>
+    <t>Je transfert le MLD que j'avais réalisé précedemment sur papier sur MySQL Workbench et j'y ajoute les champs auquel je n'avais pas pensé lors de la première conception du MLD et du MCD.</t>
+  </si>
+  <si>
+    <t>Définition des activités possible, qui seront par la suite détaillée dans un diagramme UML</t>
+  </si>
+  <si>
+    <t>Ajout d'endpoints à l'API suite à la mise à jour du MLD</t>
   </si>
 </sst>
 </file>
@@ -464,8 +482,8 @@
   <dimension ref="A1:E144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,24 +852,66 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="D24" s="2"/>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="2">
+        <v>43509</v>
+      </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="D26" s="2"/>
+    <row r="25" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25">
+        <v>1.5</v>
+      </c>
+      <c r="D25" s="2">
+        <v>43510</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2">
+        <v>43510</v>
+      </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="D27" s="2"/>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="2">
+        <v>43510</v>
+      </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added new endpoints documentation, Added Use case diagram
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>Ajout d'endpoints à l'API suite à la mise à jour du MLD</t>
+  </si>
+  <si>
+    <t>Je créer des diagrammes UML d'activité pour décrire le fonctionnement de l'API</t>
   </si>
 </sst>
 </file>
@@ -481,9 +484,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +494,7 @@
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="53.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -914,9 +917,19 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="D28" s="2"/>
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" s="2">
+        <v>43510</v>
+      </c>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated RapportDeTravail and JournalDeBord
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0DBA0C-3425-49BA-81B5-2821424EDF8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -154,12 +155,21 @@
   </si>
   <si>
     <t>Je créer des diagrammes UML d'activité pour décrire le fonctionnement de l'API</t>
+  </si>
+  <si>
+    <t>J'installe les différents composants nécessaire au bon fonctionnement du serveur</t>
+  </si>
+  <si>
+    <t>Documentation de l'installation et de la configuration du Raspberry Pi</t>
+  </si>
+  <si>
+    <t>Installation du Raspberry Pi et configuration de fail2ban, ufw, ssh, nodejs et npm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
@@ -481,24 +491,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="53.28515625" customWidth="1"/>
+    <col min="5" max="5" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -515,7 +525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -530,7 +540,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -545,7 +555,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -560,7 +570,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -575,7 +585,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -590,7 +600,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -607,7 +617,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -622,7 +632,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -639,7 +649,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -656,7 +666,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -671,7 +681,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -688,7 +698,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -703,7 +713,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -718,7 +728,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -733,7 +743,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -748,7 +758,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -763,7 +773,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -778,7 +788,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -793,7 +803,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -808,7 +818,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
@@ -823,7 +833,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -838,7 +848,7 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
@@ -855,7 +865,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
@@ -870,7 +880,7 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
@@ -887,7 +897,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
@@ -902,7 +912,7 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
@@ -917,7 +927,7 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
@@ -932,559 +942,581 @@
       </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="D30" s="2"/>
+    <row r="29" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2">
+        <v>43514</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2">
+        <v>43514</v>
+      </c>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
       <c r="D31" s="2"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
       <c r="D32" s="2"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="D33" s="2"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="D34" s="2"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="D35" s="2"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="D36" s="2"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
       <c r="D37" s="2"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="D38" s="2"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="D39" s="2"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
       <c r="D40" s="2"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="D41" s="2"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="D42" s="2"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="D43" s="2"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="D44" s="2"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
       <c r="D45" s="2"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
       <c r="D46" s="2"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="D47" s="2"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="D48" s="2"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
       <c r="D49" s="2"/>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
       <c r="D50" s="2"/>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
       <c r="D51" s="2"/>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
       <c r="D52" s="2"/>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
       <c r="D53" s="2"/>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="D54" s="2"/>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B55" s="1"/>
       <c r="D55" s="2"/>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B56" s="1"/>
       <c r="D56" s="2"/>
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B57" s="1"/>
       <c r="D57" s="2"/>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58" s="1"/>
       <c r="D58" s="2"/>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B59" s="1"/>
       <c r="D59" s="2"/>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B60" s="1"/>
       <c r="D60" s="2"/>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B61" s="1"/>
       <c r="D61" s="2"/>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B62" s="1"/>
       <c r="D62" s="2"/>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B63" s="1"/>
       <c r="D63" s="2"/>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B64" s="1"/>
       <c r="D64" s="2"/>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B65" s="1"/>
       <c r="D65" s="2"/>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B66" s="1"/>
       <c r="D66" s="2"/>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67" s="1"/>
       <c r="D67" s="2"/>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B68" s="1"/>
       <c r="D68" s="2"/>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B69" s="1"/>
       <c r="D69" s="2"/>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B70" s="1"/>
       <c r="D70" s="2"/>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B71" s="1"/>
       <c r="D71" s="2"/>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B72" s="1"/>
       <c r="D72" s="2"/>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B73" s="1"/>
       <c r="D73" s="2"/>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B74" s="1"/>
       <c r="D74" s="2"/>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B75" s="1"/>
       <c r="D75" s="2"/>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B76" s="1"/>
       <c r="D76" s="2"/>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B77" s="1"/>
       <c r="D77" s="2"/>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B78" s="1"/>
       <c r="D78" s="2"/>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B79" s="1"/>
       <c r="D79" s="2"/>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B80" s="1"/>
       <c r="D80" s="2"/>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B81" s="1"/>
       <c r="D81" s="2"/>
       <c r="E81" s="1"/>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B82" s="1"/>
       <c r="D82" s="2"/>
       <c r="E82" s="1"/>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B83" s="1"/>
       <c r="D83" s="2"/>
       <c r="E83" s="1"/>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B84" s="1"/>
       <c r="D84" s="2"/>
       <c r="E84" s="1"/>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B85" s="1"/>
       <c r="D85" s="2"/>
       <c r="E85" s="1"/>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B86" s="1"/>
       <c r="D86" s="2"/>
       <c r="E86" s="1"/>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B87" s="1"/>
       <c r="D87" s="2"/>
       <c r="E87" s="1"/>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B88" s="1"/>
       <c r="D88" s="2"/>
       <c r="E88" s="1"/>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B89" s="1"/>
       <c r="D89" s="2"/>
       <c r="E89" s="1"/>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B90" s="1"/>
       <c r="D90" s="2"/>
       <c r="E90" s="1"/>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B91" s="1"/>
       <c r="D91" s="2"/>
       <c r="E91" s="1"/>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B92" s="1"/>
       <c r="D92" s="2"/>
       <c r="E92" s="1"/>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B93" s="1"/>
       <c r="D93" s="2"/>
       <c r="E93" s="1"/>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B94" s="1"/>
       <c r="D94" s="2"/>
       <c r="E94" s="1"/>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B95" s="1"/>
       <c r="D95" s="2"/>
       <c r="E95" s="1"/>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B96" s="1"/>
       <c r="D96" s="2"/>
       <c r="E96" s="1"/>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B97" s="1"/>
       <c r="D97" s="2"/>
       <c r="E97" s="1"/>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B98" s="1"/>
       <c r="D98" s="2"/>
       <c r="E98" s="1"/>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B99" s="1"/>
       <c r="D99" s="2"/>
       <c r="E99" s="1"/>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B100" s="1"/>
       <c r="D100" s="2"/>
       <c r="E100" s="1"/>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B101" s="1"/>
       <c r="D101" s="2"/>
       <c r="E101" s="1"/>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B102" s="1"/>
       <c r="D102" s="2"/>
       <c r="E102" s="1"/>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B103" s="1"/>
       <c r="D103" s="2"/>
       <c r="E103" s="1"/>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B104" s="1"/>
       <c r="D104" s="2"/>
       <c r="E104" s="1"/>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B105" s="1"/>
       <c r="D105" s="2"/>
       <c r="E105" s="1"/>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B106" s="1"/>
       <c r="D106" s="2"/>
       <c r="E106" s="1"/>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B107" s="1"/>
       <c r="D107" s="2"/>
       <c r="E107" s="1"/>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B108" s="1"/>
       <c r="D108" s="2"/>
       <c r="E108" s="1"/>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B109" s="1"/>
       <c r="D109" s="2"/>
       <c r="E109" s="1"/>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B110" s="1"/>
       <c r="D110" s="2"/>
       <c r="E110" s="1"/>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B111" s="1"/>
       <c r="D111" s="2"/>
       <c r="E111" s="1"/>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B112" s="1"/>
       <c r="D112" s="2"/>
       <c r="E112" s="1"/>
     </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B113" s="1"/>
       <c r="D113" s="2"/>
       <c r="E113" s="1"/>
     </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B114" s="1"/>
       <c r="D114" s="2"/>
       <c r="E114" s="1"/>
     </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B115" s="1"/>
       <c r="D115" s="2"/>
       <c r="E115" s="1"/>
     </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B116" s="1"/>
       <c r="D116" s="2"/>
       <c r="E116" s="1"/>
     </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B117" s="1"/>
       <c r="D117" s="2"/>
       <c r="E117" s="1"/>
     </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B118" s="1"/>
       <c r="D118" s="2"/>
       <c r="E118" s="1"/>
     </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B119" s="1"/>
       <c r="D119" s="2"/>
       <c r="E119" s="1"/>
     </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B120" s="1"/>
       <c r="D120" s="2"/>
       <c r="E120" s="1"/>
     </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B121" s="1"/>
       <c r="D121" s="2"/>
       <c r="E121" s="1"/>
     </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B122" s="1"/>
       <c r="D122" s="2"/>
       <c r="E122" s="1"/>
     </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B123" s="1"/>
       <c r="D123" s="2"/>
       <c r="E123" s="1"/>
     </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B124" s="1"/>
       <c r="D124" s="2"/>
       <c r="E124" s="1"/>
     </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B125" s="1"/>
       <c r="D125" s="2"/>
       <c r="E125" s="1"/>
     </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B126" s="1"/>
       <c r="D126" s="2"/>
       <c r="E126" s="1"/>
     </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B127" s="1"/>
       <c r="D127" s="2"/>
     </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B128" s="1"/>
       <c r="D128" s="2"/>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B129" s="1"/>
       <c r="D129" s="2"/>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B130" s="1"/>
       <c r="D130" s="2"/>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B131" s="1"/>
       <c r="D131" s="2"/>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B132" s="1"/>
       <c r="D132" s="2"/>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B133" s="1"/>
       <c r="D133" s="2"/>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B134" s="1"/>
       <c r="D134" s="2"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B135" s="1"/>
       <c r="D135" s="2"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B136" s="1"/>
       <c r="D136" s="2"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B137" s="1"/>
       <c r="D137" s="2"/>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B138" s="1"/>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B139" s="1"/>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B140" s="1"/>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B141" s="1"/>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B142" s="1"/>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B143" s="1"/>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B144" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added first use case
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0DBA0C-3425-49BA-81B5-2821424EDF8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -164,12 +163,18 @@
   </si>
   <si>
     <t>Installation du Raspberry Pi et configuration de fail2ban, ufw, ssh, nodejs et npm</t>
+  </si>
+  <si>
+    <t>Je réalise des diagrammes de flux des différentes activités</t>
+  </si>
+  <si>
+    <t>Rédaction du premier use case, le use case du visiteur qui créer un compte</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
@@ -491,24 +496,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E144"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="53.33203125" customWidth="1"/>
+    <col min="5" max="5" width="53.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -525,7 +530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -540,7 +545,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -555,7 +560,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -570,7 +575,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -585,7 +590,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -600,7 +605,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -617,7 +622,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -632,7 +637,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -649,7 +654,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -666,7 +671,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -681,7 +686,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -698,7 +703,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -713,7 +718,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -728,7 +733,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -743,7 +748,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -758,7 +763,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -773,7 +778,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -788,7 +793,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
@@ -803,7 +808,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -818,7 +823,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
@@ -833,7 +838,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -848,7 +853,7 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
@@ -865,7 +870,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
@@ -880,7 +885,7 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
@@ -897,7 +902,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
@@ -912,7 +917,7 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
@@ -927,7 +932,7 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
@@ -942,582 +947,612 @@
       </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D29" s="2">
-        <v>43514</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>43511</v>
+      </c>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" s="2">
+        <v>43511</v>
+      </c>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" s="2">
         <v>43514</v>
       </c>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="1"/>
-      <c r="D32" s="2"/>
+      <c r="E31" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2">
+        <v>43514</v>
+      </c>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="D33" s="2"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="D34" s="2"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="D35" s="2"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="D36" s="2"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="D37" s="2"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="D38" s="2"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="D39" s="2"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="D40" s="2"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="D41" s="2"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="D42" s="2"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="D43" s="2"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="D44" s="2"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="D45" s="2"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="D46" s="2"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="D47" s="2"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="D48" s="2"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="D49" s="2"/>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="D50" s="2"/>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="D51" s="2"/>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="D52" s="2"/>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="D53" s="2"/>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="D54" s="2"/>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="D55" s="2"/>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="D56" s="2"/>
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="D57" s="2"/>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="D58" s="2"/>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="D59" s="2"/>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="D60" s="2"/>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="D61" s="2"/>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="D62" s="2"/>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="D63" s="2"/>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="D64" s="2"/>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="D65" s="2"/>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="D66" s="2"/>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
       <c r="D67" s="2"/>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="D68" s="2"/>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="D69" s="2"/>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="D70" s="2"/>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="D71" s="2"/>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="D72" s="2"/>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="D73" s="2"/>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="D74" s="2"/>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
       <c r="D75" s="2"/>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="D76" s="2"/>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="D77" s="2"/>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="D78" s="2"/>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
       <c r="D79" s="2"/>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="D80" s="2"/>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="D81" s="2"/>
       <c r="E81" s="1"/>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="D82" s="2"/>
       <c r="E82" s="1"/>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="D83" s="2"/>
       <c r="E83" s="1"/>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="D84" s="2"/>
       <c r="E84" s="1"/>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="D85" s="2"/>
       <c r="E85" s="1"/>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
       <c r="D86" s="2"/>
       <c r="E86" s="1"/>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="D87" s="2"/>
       <c r="E87" s="1"/>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
       <c r="D88" s="2"/>
       <c r="E88" s="1"/>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
       <c r="D89" s="2"/>
       <c r="E89" s="1"/>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="1"/>
       <c r="D90" s="2"/>
       <c r="E90" s="1"/>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
       <c r="D91" s="2"/>
       <c r="E91" s="1"/>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
       <c r="D92" s="2"/>
       <c r="E92" s="1"/>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="1"/>
       <c r="D93" s="2"/>
       <c r="E93" s="1"/>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
       <c r="D94" s="2"/>
       <c r="E94" s="1"/>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="1"/>
       <c r="D95" s="2"/>
       <c r="E95" s="1"/>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
       <c r="D96" s="2"/>
       <c r="E96" s="1"/>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
       <c r="D97" s="2"/>
       <c r="E97" s="1"/>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="D98" s="2"/>
       <c r="E98" s="1"/>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
       <c r="D99" s="2"/>
       <c r="E99" s="1"/>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
       <c r="D100" s="2"/>
       <c r="E100" s="1"/>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B101" s="1"/>
       <c r="D101" s="2"/>
       <c r="E101" s="1"/>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B102" s="1"/>
       <c r="D102" s="2"/>
       <c r="E102" s="1"/>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B103" s="1"/>
       <c r="D103" s="2"/>
       <c r="E103" s="1"/>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B104" s="1"/>
       <c r="D104" s="2"/>
       <c r="E104" s="1"/>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="D105" s="2"/>
       <c r="E105" s="1"/>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="D106" s="2"/>
       <c r="E106" s="1"/>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="D107" s="2"/>
       <c r="E107" s="1"/>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="D108" s="2"/>
       <c r="E108" s="1"/>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B109" s="1"/>
       <c r="D109" s="2"/>
       <c r="E109" s="1"/>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
       <c r="D110" s="2"/>
       <c r="E110" s="1"/>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B111" s="1"/>
       <c r="D111" s="2"/>
       <c r="E111" s="1"/>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B112" s="1"/>
       <c r="D112" s="2"/>
       <c r="E112" s="1"/>
     </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B113" s="1"/>
       <c r="D113" s="2"/>
       <c r="E113" s="1"/>
     </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B114" s="1"/>
       <c r="D114" s="2"/>
       <c r="E114" s="1"/>
     </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B115" s="1"/>
       <c r="D115" s="2"/>
       <c r="E115" s="1"/>
     </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B116" s="1"/>
       <c r="D116" s="2"/>
       <c r="E116" s="1"/>
     </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B117" s="1"/>
       <c r="D117" s="2"/>
       <c r="E117" s="1"/>
     </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B118" s="1"/>
       <c r="D118" s="2"/>
       <c r="E118" s="1"/>
     </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B119" s="1"/>
       <c r="D119" s="2"/>
       <c r="E119" s="1"/>
     </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B120" s="1"/>
       <c r="D120" s="2"/>
       <c r="E120" s="1"/>
     </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B121" s="1"/>
       <c r="D121" s="2"/>
       <c r="E121" s="1"/>
     </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B122" s="1"/>
       <c r="D122" s="2"/>
       <c r="E122" s="1"/>
     </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B123" s="1"/>
       <c r="D123" s="2"/>
       <c r="E123" s="1"/>
     </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B124" s="1"/>
       <c r="D124" s="2"/>
       <c r="E124" s="1"/>
     </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B125" s="1"/>
       <c r="D125" s="2"/>
       <c r="E125" s="1"/>
     </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B126" s="1"/>
       <c r="D126" s="2"/>
       <c r="E126" s="1"/>
     </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B127" s="1"/>
       <c r="D127" s="2"/>
-    </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E127" s="1"/>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B128" s="1"/>
       <c r="D128" s="2"/>
-    </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E128" s="1"/>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" s="1"/>
       <c r="D129" s="2"/>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="1"/>
       <c r="D130" s="2"/>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" s="1"/>
       <c r="D131" s="2"/>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" s="1"/>
       <c r="D132" s="2"/>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" s="1"/>
       <c r="D133" s="2"/>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" s="1"/>
       <c r="D134" s="2"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" s="1"/>
       <c r="D135" s="2"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B136" s="1"/>
       <c r="D136" s="2"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" s="1"/>
       <c r="D137" s="2"/>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" s="1"/>
-    </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D138" s="2"/>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" s="1"/>
-    </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D139" s="2"/>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B140" s="1"/>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B141" s="1"/>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B142" s="1"/>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B143" s="1"/>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B144" s="1"/>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B145" s="1"/>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B146" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added first version of API user and Token Endpoints
-Added GET user endpoint
-Added GET user/:id endpoint
-Added POST user/:id endpoint
-Added PUT user endpoint
-Added GET token endpoint
-Added support for mysql databases
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Création d'un nouvel utilisateur SQL et exécution du script de création des tables sur le serveur</t>
   </si>
   <si>
-    <t>Création du endpoint API qui permet de sélectionner un utilisateur</t>
-  </si>
-  <si>
     <t>Liaison de NodeJS et de la base de données MySQL</t>
   </si>
   <si>
@@ -193,6 +190,27 @@
   </si>
   <si>
     <t>Conception du module d'authentification, explication du choix technologique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réalisation </t>
+  </si>
+  <si>
+    <t>Création du endpoint API qui permet de sélectionner des utilisateurs</t>
+  </si>
+  <si>
+    <t>Finalisation du endpoint de selection des utilisateurs et création du endpoints permettant de sélectionner un seul utilisateur</t>
+  </si>
+  <si>
+    <t>Création du endpoint de gestion des tokens et réalisation de toute la logique de création de tokens</t>
+  </si>
+  <si>
+    <t>Tests sur le endpoint de récupération de tokens pour trouver des bugs. Un bug était présent lorsque aucun paramètre n'était envoyé avec la requête</t>
+  </si>
+  <si>
+    <t>Mise à jour du script SQL de création de la base de données pour rendre le script compatible avec les anciennes versions de MYSQL</t>
+  </si>
+  <si>
+    <t>Refactoring de la gestion des JWT pour améliorer la lisibilité et la réutilisation du code. Création de la fonction de vérification des JWT pour authentifier les utilisateurs</t>
   </si>
 </sst>
 </file>
@@ -524,8 +542,8 @@
   <dimension ref="A1:E149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,7 +1086,7 @@
         <v>13</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C35">
         <v>0.5</v>
@@ -1083,7 +1101,7 @@
         <v>18</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C36">
         <v>0.5</v>
@@ -1128,7 +1146,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39">
         <v>0.5</v>
@@ -1143,7 +1161,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C40">
         <v>1.5</v>
@@ -1153,30 +1171,79 @@
       </c>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="D41" s="2"/>
+    <row r="41" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" s="2">
+        <v>43523</v>
+      </c>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="1"/>
-      <c r="D42" s="2"/>
+    <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42">
+        <v>2.5</v>
+      </c>
+      <c r="D42" s="2">
+        <v>43528</v>
+      </c>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
-      <c r="D43" s="2"/>
+    <row r="43" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43">
+        <v>0.75</v>
+      </c>
+      <c r="D43" s="2">
+        <v>43529</v>
+      </c>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="1"/>
-      <c r="D44" s="2"/>
+    <row r="44" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44">
+        <v>0.5</v>
+      </c>
+      <c r="D44" s="2">
+        <v>43530</v>
+      </c>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
-      <c r="D45" s="2"/>
+    <row r="45" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2">
+        <v>43530</v>
+      </c>
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added work done today
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88906174-6F90-4F78-982E-402648398620}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A269D5-A987-43AB-A32F-1DE1313E9C42}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="82">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t>Tests des Uses cases sur la ressources token, correction des bugs découverts</t>
+  </si>
+  <si>
+    <t>Continuation du développement du endpoint d'activité, debug de la création d'activtié qui posait problème</t>
   </si>
 </sst>
 </file>
@@ -594,8 +597,8 @@
   <dimension ref="A1:E150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,10 +1541,19 @@
       </c>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="D62" s="2"/>
+    <row r="62" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C62">
+        <v>1.5</v>
+      </c>
+      <c r="D62" s="2">
+        <v>43537</v>
+      </c>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated with work done today
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A269D5-A987-43AB-A32F-1DE1313E9C42}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2DBCC5-BD08-4893-8E23-6B6F6AB9F3C9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="87">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -266,6 +266,21 @@
   </si>
   <si>
     <t>Continuation du développement du endpoint d'activité, debug de la création d'activtié qui posait problème</t>
+  </si>
+  <si>
+    <t>Création du endpoint de sélection d'activité</t>
+  </si>
+  <si>
+    <t>Création du endpoint de création de type d'activité ainsi que de sélection du type d'activité</t>
+  </si>
+  <si>
+    <t>Création de la page de login de l'interface web d'administration à l'aide des maquettes graphique réalisé précédement</t>
+  </si>
+  <si>
+    <t>Déploiement de la page de login sur le serveur node, déplacement de tout l'api et adalptation du code pour prendre en compte les changements</t>
+  </si>
+  <si>
+    <t>Continuation du debug de l'endpoint d'activité, des bugs étaient présent lors de l'insertion d'une nouvelle activité car la contrainte de clé étrangère du type d'activité n'était pas satisfaite</t>
   </si>
 </sst>
 </file>
@@ -594,11 +609,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:E151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
+      <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,92 +1571,142 @@
       </c>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="1"/>
-      <c r="D63" s="2"/>
+    <row r="63" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" s="2">
+        <v>43538</v>
+      </c>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="1"/>
-      <c r="D64" s="2"/>
+    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64">
+        <v>1.5</v>
+      </c>
+      <c r="D64" s="2">
+        <v>43538</v>
+      </c>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="1"/>
-      <c r="D65" s="2"/>
+    <row r="65" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65">
+        <v>1.5</v>
+      </c>
+      <c r="D65" s="2">
+        <v>43538</v>
+      </c>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="1"/>
-      <c r="D66" s="2"/>
+    <row r="66" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66" s="2">
+        <v>43538</v>
+      </c>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="1"/>
-      <c r="D67" s="2"/>
+    <row r="67" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C67">
+        <v>1.5</v>
+      </c>
+      <c r="D67" s="2">
+        <v>43538</v>
+      </c>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="D68" s="2"/>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="D69" s="2"/>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="D70" s="2"/>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="D71" s="2"/>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="D72" s="2"/>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="D73" s="2"/>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="D74" s="2"/>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
       <c r="D75" s="2"/>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="D76" s="2"/>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="D77" s="2"/>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="D78" s="2"/>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
       <c r="D79" s="2"/>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="D80" s="2"/>
       <c r="E80" s="1"/>
@@ -1909,6 +1974,7 @@
     <row r="133" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B133" s="1"/>
       <c r="D133" s="2"/>
+      <c r="E133" s="1"/>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B134" s="1"/>
@@ -1952,6 +2018,7 @@
     </row>
     <row r="144" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B144" s="1"/>
+      <c r="D144" s="2"/>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" s="1"/>
@@ -1970,6 +2037,9 @@
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" s="1"/>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B151" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated with latest tasks
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2DBCC5-BD08-4893-8E23-6B6F6AB9F3C9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63245024-70FC-4F1E-BDDC-E6CD25A9EB93}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -281,6 +281,15 @@
   </si>
   <si>
     <t>Continuation du debug de l'endpoint d'activité, des bugs étaient présent lors de l'insertion d'une nouvelle activité car la contrainte de clé étrangère du type d'activité n'était pas satisfaite</t>
+  </si>
+  <si>
+    <t>Ajout d'une description aux Entités pour justifier les cardinalités</t>
+  </si>
+  <si>
+    <t>Modifications des CCS sur la page de login pour la validation des champs, modification du champ email en type "email", récupération du token et sauvegarde de celui-ci dans un cookie</t>
+  </si>
+  <si>
+    <t>Modification du Wireframe de la page de login pour y ajouter le retour d'erreur, ajout du Wireframe à la documentation</t>
   </si>
 </sst>
 </file>
@@ -609,11 +618,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,24 +1655,64 @@
       </c>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="1"/>
-      <c r="D68" s="2"/>
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68" s="2">
+        <v>43539</v>
+      </c>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="1"/>
-      <c r="D69" s="2"/>
+    <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C69">
+        <v>0.5</v>
+      </c>
+      <c r="D69" s="2">
+        <v>43540</v>
+      </c>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="1"/>
-      <c r="D70" s="2"/>
+    <row r="70" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70" s="2">
+        <v>43540</v>
+      </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B71" s="1"/>
-      <c r="D71" s="2"/>
+    <row r="71" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C71">
+        <v>0.5</v>
+      </c>
+      <c r="D71" s="2">
+        <v>43540</v>
+      </c>
       <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1979,6 +2028,7 @@
     <row r="134" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B134" s="1"/>
       <c r="D134" s="2"/>
+      <c r="E134" s="1"/>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B135" s="1"/>
@@ -2020,26 +2070,30 @@
       <c r="B144" s="1"/>
       <c r="D144" s="2"/>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B145" s="1"/>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D145" s="2"/>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B146" s="1"/>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B147" s="1"/>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B148" s="1"/>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B149" s="1"/>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B150" s="1"/>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B151" s="1"/>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added tasks done today
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63245024-70FC-4F1E-BDDC-E6CD25A9EB93}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801709C2-9802-41E2-8C98-CF7BE3FFC463}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="97">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -290,6 +290,27 @@
   </si>
   <si>
     <t>Modification du Wireframe de la page de login pour y ajouter le retour d'erreur, ajout du Wireframe à la documentation</t>
+  </si>
+  <si>
+    <t>Modification des marges sur la page de login. Les marges posaient des problèmes sur la version mobile de la page car elles étaient calculées par rapport à la taille du viewport</t>
+  </si>
+  <si>
+    <t>Documentation de l'utilité de mettre en place une standardisation du retour d'erreur de l'API</t>
+  </si>
+  <si>
+    <t>Réflexion sur la structure de retour de l'API ainsi que les types d'erreurs possible</t>
+  </si>
+  <si>
+    <t>Création d'une classe de gestion de réponse, modifications des actions utilisateurs pour que les méthodes retournent des Promises</t>
+  </si>
+  <si>
+    <t>Transformation des méthodes d'actions sur les activités pour que celles-ci retournent des Promises</t>
+  </si>
+  <si>
+    <t>Ajout d'une méthode de login à la classe d'actions utilisalteurs, implémentation de cette méthode lors de l'appel de l'endpoint /token</t>
+  </si>
+  <si>
+    <t>J'ai passé un peu de temps à lire la documentation sur les Promises, je n'était pas totalement au clair avec le rejet des Promises</t>
   </si>
 </sst>
 </file>
@@ -621,8 +642,8 @@
   <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,35 +1736,97 @@
       </c>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="1"/>
-      <c r="D72" s="2"/>
+    <row r="72" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C72">
+        <v>0.5</v>
+      </c>
+      <c r="D72" s="2">
+        <v>43540</v>
+      </c>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="1"/>
-      <c r="D73" s="2"/>
+    <row r="73" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C73">
+        <v>0.5</v>
+      </c>
+      <c r="D73" s="2">
+        <v>43543</v>
+      </c>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="1"/>
-      <c r="D74" s="2"/>
+    <row r="74" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C74">
+        <v>0.5</v>
+      </c>
+      <c r="D74" s="2">
+        <v>43543</v>
+      </c>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="1"/>
-      <c r="D75" s="2"/>
+    <row r="75" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C75">
+        <v>1.5</v>
+      </c>
+      <c r="D75" s="2">
+        <v>43543</v>
+      </c>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="1"/>
-      <c r="D76" s="2"/>
+    <row r="76" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C76">
+        <v>0.5</v>
+      </c>
+      <c r="D76" s="2">
+        <v>43543</v>
+      </c>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="1"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="1"/>
+    <row r="77" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77" s="2">
+        <v>43543</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>

</xml_diff>

<commit_message>
Added Authentication on Activity Analysis and Conception
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801709C2-9802-41E2-8C98-CF7BE3FFC463}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="100">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -311,12 +310,21 @@
   </si>
   <si>
     <t>J'ai passé un peu de temps à lire la documentation sur les Promises, je n'était pas totalement au clair avec le rejet des Promises</t>
+  </si>
+  <si>
+    <t>Remontée des erreurs au niveau du catch sur les controlleurs (dans le fichier app.js)</t>
+  </si>
+  <si>
+    <t>Réalisation de 2 diagrammes de séquences décrivant les principales étapes d'une requête sur le serveur</t>
+  </si>
+  <si>
+    <t>Modifications des méthodes de vérification des tokens</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
@@ -638,12 +646,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E152"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A78" sqref="A78"/>
+      <selection pane="bottomLeft" activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,19 +1836,49 @@
         <v>96</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="1"/>
-      <c r="D78" s="2"/>
+    <row r="78" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C78">
+        <v>3</v>
+      </c>
+      <c r="D78" s="2">
+        <v>43544</v>
+      </c>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="1"/>
-      <c r="D79" s="2"/>
+    <row r="79" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C79">
+        <v>1.5</v>
+      </c>
+      <c r="D79" s="2">
+        <v>43545</v>
+      </c>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="1"/>
-      <c r="D80" s="2"/>
+    <row r="80" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C80">
+        <v>1.5</v>
+      </c>
+      <c r="D80" s="2">
+        <v>43545</v>
+      </c>
       <c r="E80" s="1"/>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
@@ -2116,6 +2154,7 @@
     <row r="135" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B135" s="1"/>
       <c r="D135" s="2"/>
+      <c r="E135" s="1"/>
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B136" s="1"/>
@@ -2159,6 +2198,7 @@
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B146" s="1"/>
+      <c r="D146" s="2"/>
     </row>
     <row r="147" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B147" s="1"/>
@@ -2177,6 +2217,9 @@
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B152" s="1"/>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B153" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated with task done last week
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="102">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -319,6 +319,12 @@
   </si>
   <si>
     <t>Modifications des méthodes de vérification des tokens</t>
+  </si>
+  <si>
+    <t>Je commence à réalisé l'extration des données du fichier GPX lié à la requête de création d'activités</t>
+  </si>
+  <si>
+    <t>Ajout du endpoint permettant de récuperer toutes les activités d'un utilisateur</t>
   </si>
 </sst>
 </file>
@@ -647,11 +653,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E153"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C82" sqref="C82"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1881,82 +1887,112 @@
       </c>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="1"/>
-      <c r="D81" s="2"/>
+    <row r="81" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81" s="2">
+        <v>43546</v>
+      </c>
       <c r="E81" s="1"/>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="1"/>
-      <c r="D82" s="2"/>
+    <row r="82" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C82">
+        <v>5</v>
+      </c>
+      <c r="D82" s="2">
+        <v>43546</v>
+      </c>
       <c r="E82" s="1"/>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="1"/>
-      <c r="D83" s="2"/>
+    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C83">
+        <v>0.75</v>
+      </c>
+      <c r="D83" s="2">
+        <v>43546</v>
+      </c>
       <c r="E83" s="1"/>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="D84" s="2"/>
       <c r="E84" s="1"/>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="D85" s="2"/>
       <c r="E85" s="1"/>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
       <c r="D86" s="2"/>
       <c r="E86" s="1"/>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="D87" s="2"/>
       <c r="E87" s="1"/>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
       <c r="D88" s="2"/>
       <c r="E88" s="1"/>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
       <c r="D89" s="2"/>
       <c r="E89" s="1"/>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B90" s="1"/>
       <c r="D90" s="2"/>
       <c r="E90" s="1"/>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
       <c r="D91" s="2"/>
       <c r="E91" s="1"/>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
       <c r="D92" s="2"/>
       <c r="E92" s="1"/>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B93" s="1"/>
       <c r="D93" s="2"/>
       <c r="E93" s="1"/>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
       <c r="D94" s="2"/>
       <c r="E94" s="1"/>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B95" s="1"/>
       <c r="D95" s="2"/>
       <c r="E95" s="1"/>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
       <c r="D96" s="2"/>
       <c r="E96" s="1"/>
@@ -2159,6 +2195,7 @@
     <row r="136" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B136" s="1"/>
       <c r="D136" s="2"/>
+      <c r="E136" s="1"/>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B137" s="1"/>
@@ -2202,6 +2239,7 @@
     </row>
     <row r="147" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B147" s="1"/>
+      <c r="D147" s="2"/>
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B148" s="1"/>
@@ -2220,6 +2258,9 @@
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B153" s="1"/>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B154" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated with task done this week
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F10B1E-FB22-44F3-AA0E-6DB8FC7EBE30}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="113">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -325,12 +326,45 @@
   </si>
   <si>
     <t>Ajout du endpoint permettant de récuperer toutes les activités d'un utilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je continue d'extraire les informations du fichier GPX, je recontre quelques difficultés car le module nodejs que j'utilise (gpx-parse) ne possède pas énormément de documentation </t>
+  </si>
+  <si>
+    <t>Continuation de l'extraction des données du GPX, j'arrive désormais a créer des enregistrements dans la table des positions. J'ai commencé à ajouté les champs qui vont être calculés à la base de données</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'effectue réalisé les calculs pour les nouveaux champs de l'entité d'activité. </t>
+  </si>
+  <si>
+    <t>J'ai rencontré des problèmes avec le fichier GPX fournit par M. Glassey, un problème lors de l'exportation de celui-ci à du survenir, car les timestamps de celui-ci n'était pas correct, ce qui faussait mes résultats.</t>
+  </si>
+  <si>
+    <t>Correction d'un bug lors de la création d'activtié qui empêchait la création sans fichier gpx</t>
+  </si>
+  <si>
+    <t>Gestion de projet</t>
+  </si>
+  <si>
+    <t>Mise à jour de Trello, je prends contact avec M. Glassey pour planifier la tâche suivante. Je souhaiterai travailler sur l'authentification par token</t>
+  </si>
+  <si>
+    <t>Je me rends compte d'un besoin d'implémenter une gestion de token non-JWT pour l'interface web</t>
+  </si>
+  <si>
+    <t>J'image la forme que peut prendre ce nouveau composant au sein de l'API. Je pense ajouté une nouvelle table gérant les token de session</t>
+  </si>
+  <si>
+    <t>Mise à jour du MLD, mise à jour du schéma de la base de données</t>
+  </si>
+  <si>
+    <t>Mise à jour du Journal de bord</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
@@ -652,12 +686,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E81" sqref="E81"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1932,49 +1966,141 @@
       </c>
       <c r="E83" s="1"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="1"/>
-      <c r="D84" s="2"/>
+    <row r="84" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C84">
+        <v>0.75</v>
+      </c>
+      <c r="D84" s="2">
+        <v>43550</v>
+      </c>
       <c r="E84" s="1"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="1"/>
-      <c r="D85" s="2"/>
+    <row r="85" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C85">
+        <v>1.5</v>
+      </c>
+      <c r="D85" s="2">
+        <v>43551</v>
+      </c>
       <c r="E85" s="1"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="1"/>
-      <c r="D86" s="2"/>
-      <c r="E86" s="1"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="1"/>
-      <c r="D87" s="2"/>
+    <row r="86" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C86">
+        <v>3</v>
+      </c>
+      <c r="D86" s="2">
+        <v>43551</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87" s="2">
+        <v>43552</v>
+      </c>
       <c r="E87" s="1"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="1"/>
-      <c r="D88" s="2"/>
+    <row r="88" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C88">
+        <v>0.5</v>
+      </c>
+      <c r="D88" s="2">
+        <v>43552</v>
+      </c>
       <c r="E88" s="1"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B89" s="1"/>
-      <c r="D89" s="2"/>
+    <row r="89" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C89">
+        <v>0.5</v>
+      </c>
+      <c r="D89" s="2">
+        <v>43552</v>
+      </c>
       <c r="E89" s="1"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="1"/>
-      <c r="D90" s="2"/>
+    <row r="90" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90" s="2">
+        <v>43552</v>
+      </c>
       <c r="E90" s="1"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B91" s="1"/>
-      <c r="D91" s="2"/>
+    <row r="91" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91" s="2">
+        <v>43552</v>
+      </c>
       <c r="E91" s="1"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="1"/>
-      <c r="D92" s="2"/>
+      <c r="A92" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C92">
+        <v>0.5</v>
+      </c>
+      <c r="D92" s="2">
+        <v>76424</v>
+      </c>
       <c r="E92" s="1"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated documentation, started resume
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F10B1E-FB22-44F3-AA0E-6DB8FC7EBE30}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5C5BF1-009B-494B-AF64-8BC563A4EB80}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="115">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -359,6 +359,12 @@
   </si>
   <si>
     <t>Mise à jour du Journal de bord</t>
+  </si>
+  <si>
+    <t>Mise en place du nouveau système de gestion des token et incorporation de celui-ci sur l'interface web</t>
+  </si>
+  <si>
+    <t>Définition des objectifs atteint et non-atteint. Détails des points m'ayant posé des problèmes particuliers</t>
   </si>
 </sst>
 </file>
@@ -691,7 +697,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B86" sqref="B86"/>
+      <selection pane="bottomLeft" activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2099,18 +2105,38 @@
         <v>0.5</v>
       </c>
       <c r="D92" s="2">
-        <v>76424</v>
+        <v>43552</v>
       </c>
       <c r="E92" s="1"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="1"/>
-      <c r="D93" s="2"/>
+    <row r="93" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C93">
+        <v>4.5</v>
+      </c>
+      <c r="D93" s="2">
+        <v>43553</v>
+      </c>
       <c r="E93" s="1"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B94" s="1"/>
-      <c r="D94" s="2"/>
+    <row r="94" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94" s="2">
+        <v>43557</v>
+      </c>
       <c r="E94" s="1"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated documentation, fixed use cases and senarios, added missing scenarios, updated JournalDeBord, Signed MLD
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F5FF25-B2C1-4F87-8F69-1BAEA76A61E7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="118">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -367,12 +368,18 @@
   </si>
   <si>
     <t xml:space="preserve">Continuation de la conclusion </t>
+  </si>
+  <si>
+    <t>Documentation du code aux endroits où j'estimais qu'il y avait un manque de clarté</t>
+  </si>
+  <si>
+    <t>Vérification de la présence de tous les use cases , clarification de certains use cases / scénarios. Ajout de scénarios manquant + tests sur l'API</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
@@ -694,12 +701,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D96" sqref="D96"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2156,87 +2163,107 @@
       </c>
       <c r="E95" s="1"/>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B96" s="1"/>
-      <c r="D96" s="2"/>
+    <row r="96" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96" s="2">
+        <v>43558</v>
+      </c>
       <c r="E96" s="1"/>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B97" s="1"/>
-      <c r="D97" s="2"/>
+    <row r="97" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C97">
+        <v>2</v>
+      </c>
+      <c r="D97" s="2">
+        <v>43558</v>
+      </c>
       <c r="E97" s="1"/>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="D98" s="2"/>
       <c r="E98" s="1"/>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
       <c r="D99" s="2"/>
       <c r="E99" s="1"/>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
       <c r="D100" s="2"/>
       <c r="E100" s="1"/>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B101" s="1"/>
       <c r="D101" s="2"/>
       <c r="E101" s="1"/>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B102" s="1"/>
       <c r="D102" s="2"/>
       <c r="E102" s="1"/>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B103" s="1"/>
       <c r="D103" s="2"/>
       <c r="E103" s="1"/>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B104" s="1"/>
       <c r="D104" s="2"/>
       <c r="E104" s="1"/>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="D105" s="2"/>
       <c r="E105" s="1"/>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="D106" s="2"/>
       <c r="E106" s="1"/>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="D107" s="2"/>
       <c r="E107" s="1"/>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="D108" s="2"/>
       <c r="E108" s="1"/>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B109" s="1"/>
       <c r="D109" s="2"/>
       <c r="E109" s="1"/>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
       <c r="D110" s="2"/>
       <c r="E110" s="1"/>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B111" s="1"/>
       <c r="D111" s="2"/>
       <c r="E111" s="1"/>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B112" s="1"/>
       <c r="D112" s="2"/>
       <c r="E112" s="1"/>

</xml_diff>

<commit_message>
Added PHILIBERT_ManuelInstallation, Finalized RapportDeTravail
</commit_message>
<xml_diff>
--- a/documentation/PHILIBERT_JournalDeBord.xlsx
+++ b/documentation/PHILIBERT_JournalDeBord.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F5FF25-B2C1-4F87-8F69-1BAEA76A61E7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="120">
   <si>
     <t>Type d'activité</t>
   </si>
@@ -97,9 +96,6 @@
     <t>Conception du premier MLD, des changements auront surement lieu</t>
   </si>
   <si>
-    <t>Acquisition de connaisances</t>
-  </si>
-  <si>
     <t>Lecture du cahier des charges du Pré-TPI fournit par M. Glassey</t>
   </si>
   <si>
@@ -265,9 +261,6 @@
     <t>Tests des Uses cases sur la ressources token, correction des bugs découverts</t>
   </si>
   <si>
-    <t>Continuation du développement du endpoint d'activité, debug de la création d'activtié qui posait problème</t>
-  </si>
-  <si>
     <t>Création du endpoint de sélection d'activité</t>
   </si>
   <si>
@@ -374,12 +367,24 @@
   </si>
   <si>
     <t>Vérification de la présence de tous les use cases , clarification de certains use cases / scénarios. Ajout de scénarios manquant + tests sur l'API</t>
+  </si>
+  <si>
+    <t>Finalisation du résumé</t>
+  </si>
+  <si>
+    <t>Écriture des use cases et scénarios pour la gestion des activités</t>
+  </si>
+  <si>
+    <t>Continuation du développement du endpoint d'activité, debug de la création d'activité qui posait problème</t>
+  </si>
+  <si>
+    <t>Finalisation et relecture de la documentation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
@@ -701,12 +706,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E154"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +861,7 @@
         <v>43503</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -925,10 +930,10 @@
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -943,7 +948,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15">
         <v>0.5</v>
@@ -958,7 +963,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16">
         <v>0.5</v>
@@ -973,7 +978,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17">
         <v>0.5</v>
@@ -988,7 +993,7 @@
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18">
         <v>1.5</v>
@@ -1003,7 +1008,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19">
         <v>0.5</v>
@@ -1018,7 +1023,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20">
         <v>0.5</v>
@@ -1033,7 +1038,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21">
         <v>0.5</v>
@@ -1048,7 +1053,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22">
         <v>0.5</v>
@@ -1063,7 +1068,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23">
         <v>1.5</v>
@@ -1072,15 +1077,15 @@
         <v>43509</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="C24">
         <v>0.5</v>
@@ -1095,7 +1100,7 @@
         <v>18</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25">
         <v>1.5</v>
@@ -1104,7 +1109,7 @@
         <v>43510</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1112,7 +1117,7 @@
         <v>18</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1127,7 +1132,7 @@
         <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27">
         <v>0.5</v>
@@ -1142,7 +1147,7 @@
         <v>18</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -1157,7 +1162,7 @@
         <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29">
         <v>4</v>
@@ -1172,7 +1177,7 @@
         <v>18</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1184,19 +1189,19 @@
     </row>
     <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31" s="2">
         <v>43514</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1204,7 +1209,7 @@
         <v>11</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1219,7 +1224,7 @@
         <v>13</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1234,7 +1239,7 @@
         <v>11</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C34">
         <v>0.5</v>
@@ -1249,7 +1254,7 @@
         <v>13</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C35">
         <v>0.5</v>
@@ -1264,7 +1269,7 @@
         <v>18</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36">
         <v>0.5</v>
@@ -1276,10 +1281,10 @@
     </row>
     <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37">
         <v>0.5</v>
@@ -1291,10 +1296,10 @@
     </row>
     <row r="38" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -1306,10 +1311,10 @@
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C39">
         <v>0.5</v>
@@ -1321,10 +1326,10 @@
     </row>
     <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C40">
         <v>1.5</v>
@@ -1336,10 +1341,10 @@
     </row>
     <row r="41" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -1351,10 +1356,10 @@
     </row>
     <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42">
         <v>2.5</v>
@@ -1366,10 +1371,10 @@
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C43">
         <v>0.5</v>
@@ -1381,10 +1386,10 @@
     </row>
     <row r="44" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C44">
         <v>0.75</v>
@@ -1396,10 +1401,10 @@
     </row>
     <row r="45" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C45">
         <v>0.5</v>
@@ -1411,10 +1416,10 @@
     </row>
     <row r="46" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -1426,10 +1431,10 @@
     </row>
     <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C47">
         <v>2</v>
@@ -1441,10 +1446,10 @@
     </row>
     <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -1456,10 +1461,10 @@
     </row>
     <row r="49" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C49">
         <v>1.5</v>
@@ -1474,7 +1479,7 @@
         <v>11</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C50">
         <v>0.5</v>
@@ -1486,10 +1491,10 @@
     </row>
     <row r="51" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C51">
         <v>2.5</v>
@@ -1504,10 +1509,10 @@
         <v>13</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D52" s="2">
         <v>43532</v>
@@ -1516,13 +1521,13 @@
     </row>
     <row r="53" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C53">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D53" s="2">
         <v>43532</v>
@@ -1534,7 +1539,7 @@
         <v>18</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -1549,7 +1554,7 @@
         <v>3</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C55">
         <v>0.5</v>
@@ -1564,7 +1569,7 @@
         <v>11</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C56">
         <v>0.5</v>
@@ -1579,7 +1584,7 @@
         <v>11</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C57">
         <v>0.5</v>
@@ -1594,7 +1599,7 @@
         <v>13</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C58">
         <v>0.25</v>
@@ -1609,7 +1614,7 @@
         <v>13</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C59">
         <v>0.5</v>
@@ -1624,7 +1629,7 @@
         <v>18</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C60">
         <v>0.5</v>
@@ -1636,10 +1641,10 @@
     </row>
     <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -1649,57 +1654,57 @@
       </c>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62" s="2">
+        <v>43536</v>
+      </c>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63">
         <v>1.5</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D63" s="2">
         <v>43537</v>
       </c>
-      <c r="E62" s="1"/>
-    </row>
-    <row r="63" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-      <c r="D63" s="2">
-        <v>43538</v>
-      </c>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C64">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D64" s="2">
         <v>43538</v>
       </c>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C65">
         <v>1.5</v>
@@ -1711,100 +1716,100 @@
     </row>
     <row r="66" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D66" s="2">
         <v>43538</v>
       </c>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C67">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D67" s="2">
         <v>43538</v>
       </c>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C68">
+        <v>1.5</v>
+      </c>
+      <c r="D68" s="2">
+        <v>43538</v>
+      </c>
+      <c r="E68" s="1"/>
+    </row>
+    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C68">
-        <v>1</v>
-      </c>
-      <c r="D68" s="2">
+      <c r="B69" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69" s="2">
         <v>43539</v>
       </c>
-      <c r="E68" s="1"/>
-    </row>
-    <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C69">
-        <v>0.5</v>
-      </c>
-      <c r="D69" s="2">
-        <v>43540</v>
-      </c>
-      <c r="E69" s="1"/>
-    </row>
-    <row r="70" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="B70" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D70" s="2">
         <v>43540</v>
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C71">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D71" s="2">
         <v>43540</v>
       </c>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C72">
         <v>0.5</v>
@@ -1814,27 +1819,27 @@
       </c>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C73">
+        <v>0.5</v>
+      </c>
+      <c r="D73" s="2">
+        <v>43540</v>
+      </c>
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C73">
-        <v>0.5</v>
-      </c>
-      <c r="D73" s="2">
-        <v>43543</v>
-      </c>
-      <c r="E73" s="1"/>
-    </row>
-    <row r="74" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="B74" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C74">
         <v>0.5</v>
@@ -1844,89 +1849,89 @@
       </c>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C75">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="D75" s="2">
         <v>43543</v>
       </c>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C76">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="D76" s="2">
         <v>43543</v>
       </c>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C77">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D77" s="2">
         <v>43543</v>
       </c>
-      <c r="E77" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E77" s="1"/>
+    </row>
+    <row r="78" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78" s="2">
+        <v>43543</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C79">
+        <v>3</v>
+      </c>
+      <c r="D79" s="2">
+        <v>43544</v>
+      </c>
+      <c r="E79" s="1"/>
+    </row>
+    <row r="80" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C78">
-        <v>3</v>
-      </c>
-      <c r="D78" s="2">
-        <v>43544</v>
-      </c>
-      <c r="E78" s="1"/>
-    </row>
-    <row r="79" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C79">
-        <v>1.5</v>
-      </c>
-      <c r="D79" s="2">
-        <v>43545</v>
-      </c>
-      <c r="E79" s="1"/>
-    </row>
-    <row r="80" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="C80">
         <v>1.5</v>
@@ -1936,134 +1941,134 @@
       </c>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C81">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D81" s="2">
-        <v>43546</v>
+        <v>43545</v>
       </c>
       <c r="E81" s="1"/>
     </row>
-    <row r="82" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C82">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D82" s="2">
         <v>43546</v>
       </c>
       <c r="E82" s="1"/>
     </row>
-    <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="C83">
-        <v>0.75</v>
+        <v>5</v>
       </c>
       <c r="D83" s="2">
         <v>43546</v>
       </c>
       <c r="E83" s="1"/>
     </row>
-    <row r="84" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="C84">
         <v>0.75</v>
       </c>
       <c r="D84" s="2">
-        <v>43550</v>
+        <v>43546</v>
       </c>
       <c r="E84" s="1"/>
     </row>
     <row r="85" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C85">
+        <v>0.75</v>
+      </c>
+      <c r="D85" s="2">
+        <v>43550</v>
+      </c>
+      <c r="E85" s="1"/>
+    </row>
+    <row r="86" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C86">
         <v>1.5</v>
-      </c>
-      <c r="D85" s="2">
-        <v>43551</v>
-      </c>
-      <c r="E85" s="1"/>
-    </row>
-    <row r="86" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C86">
-        <v>3</v>
       </c>
       <c r="D86" s="2">
         <v>43551</v>
       </c>
-      <c r="E86" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="E86" s="1"/>
     </row>
     <row r="87" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D87" s="2">
-        <v>43552</v>
-      </c>
-      <c r="E87" s="1"/>
-    </row>
-    <row r="88" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>43551</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C88">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D88" s="2">
         <v>43552</v>
       </c>
       <c r="E88" s="1"/>
     </row>
-    <row r="89" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C89">
         <v>0.5</v>
@@ -2073,27 +2078,27 @@
       </c>
       <c r="E89" s="1"/>
     </row>
-    <row r="90" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D90" s="2">
         <v>43552</v>
       </c>
       <c r="E90" s="1"/>
     </row>
-    <row r="91" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C91">
         <v>1</v>
@@ -2103,72 +2108,72 @@
       </c>
       <c r="E91" s="1"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C92">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D92" s="2">
         <v>43552</v>
       </c>
       <c r="E92" s="1"/>
     </row>
-    <row r="93" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C93">
-        <v>4.5</v>
+        <v>0.5</v>
       </c>
       <c r="D93" s="2">
-        <v>43553</v>
+        <v>43552</v>
       </c>
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C94">
-        <v>1</v>
+        <v>4.5</v>
       </c>
       <c r="D94" s="2">
-        <v>43557</v>
+        <v>43553</v>
       </c>
       <c r="E94" s="1"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C95">
         <v>1</v>
       </c>
       <c r="D95" s="2">
-        <v>43558</v>
+        <v>43557</v>
       </c>
       <c r="E95" s="1"/>
     </row>
-    <row r="96" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -2178,34 +2183,64 @@
       </c>
       <c r="E96" s="1"/>
     </row>
-    <row r="97" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D97" s="2">
         <v>43558</v>
       </c>
       <c r="E97" s="1"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B98" s="1"/>
-      <c r="D98" s="2"/>
+    <row r="98" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C98">
+        <v>2</v>
+      </c>
+      <c r="D98" s="2">
+        <v>43558</v>
+      </c>
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B99" s="1"/>
-      <c r="D99" s="2"/>
+      <c r="A99" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99" s="2">
+        <v>43559</v>
+      </c>
       <c r="E99" s="1"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B100" s="1"/>
-      <c r="D100" s="2"/>
+    <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C100">
+        <v>4</v>
+      </c>
+      <c r="D100" s="2">
+        <v>43559</v>
+      </c>
       <c r="E100" s="1"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2391,6 +2426,7 @@
     <row r="137" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B137" s="1"/>
       <c r="D137" s="2"/>
+      <c r="E137" s="1"/>
     </row>
     <row r="138" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B138" s="1"/>
@@ -2434,6 +2470,7 @@
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B148" s="1"/>
+      <c r="D148" s="2"/>
     </row>
     <row r="149" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B149" s="1"/>
@@ -2452,6 +2489,9 @@
     </row>
     <row r="154" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B154" s="1"/>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B155" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>